<commit_message>
7 voorbeeldkaartjes aangemaakt in de excel file
</commit_message>
<xml_diff>
--- a/kaartjes.xlsx
+++ b/kaartjes.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="30" windowWidth="14355" windowHeight="10800"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
+    <sheet name="kaartjes" sheetId="2" r:id="rId1"/>
+    <sheet name="Design" sheetId="1" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="9">
   <si>
     <t>noord</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>brug</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>zuid</t>
   </si>
 </sst>
 </file>
@@ -78,7 +84,7 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="102">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -122,679 +128,34 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFD7D7D7"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
       <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="6"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1090,10 +451,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:K16" si="0">COUNTIF($B2:$E2,G$1)</f>
+        <f t="shared" ref="G2:H16" si="0">COUNTIF($B2:$E2,G$1)</f>
         <v>1</v>
       </c>
       <c r="H2">
@@ -1192,7 +704,7 @@
         <v>6</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:K28" si="1">COUNTIF($B3:$E3,F$1)</f>
+        <f t="shared" ref="F3:H28" si="1">COUNTIF($B3:$E3,F$1)</f>
         <v>2</v>
       </c>
       <c r="G3">
@@ -2269,41 +1781,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:H1 B1:E1048576">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"brug"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"land"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>"water"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:K1">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"brug"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"land"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"water"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>